<commit_message>
Adjust data to only reflect needed columns
</commit_message>
<xml_diff>
--- a/stocks.xlsx
+++ b/stocks.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="11">
   <si>
     <t>Ticker</t>
   </si>
@@ -35,12 +35,6 @@
   </si>
   <si>
     <t>Volume</t>
-  </si>
-  <si>
-    <t>Dividends</t>
-  </si>
-  <si>
-    <t>Stock Splits</t>
   </si>
   <si>
     <t>Date</t>
@@ -419,15 +413,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -447,19 +441,13 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>45538</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>163.100305814977</v>
@@ -476,19 +464,13 @@
       <c r="G2">
         <v>26533100</v>
       </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>45539</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>157.8671900814768</v>
@@ -505,19 +487,13 @@
       <c r="G3">
         <v>17410700</v>
       </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>45540</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>157.5725806698935</v>
@@ -534,19 +510,13 @@
       <c r="G4">
         <v>14139500</v>
       </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>45541</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>158.481381425261</v>
@@ -563,19 +533,13 @@
       <c r="G5">
         <v>24999100</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>45544</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>153.6300048828125</v>
@@ -592,19 +556,13 @@
       <c r="G6">
         <v>28057700</v>
       </c>
-      <c r="H6">
-        <v>0.2</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>45545</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <v>151.4499969482422</v>
@@ -621,19 +579,13 @@
       <c r="G7">
         <v>20401800</v>
       </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>45546</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>151.0899963378906</v>
@@ -650,19 +602,13 @@
       <c r="G8">
         <v>18991500</v>
       </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>45547</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>154.8099975585938</v>
@@ -679,19 +625,13 @@
       <c r="G9">
         <v>21024100</v>
       </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="2">
         <v>45548</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C10">
         <v>156.3619995117188</v>
@@ -708,19 +648,13 @@
       <c r="G10">
         <v>16733900</v>
       </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="2">
         <v>45551</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C11">
         <v>158.3300018310547</v>
@@ -737,19 +671,13 @@
       <c r="G11">
         <v>14157600</v>
       </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="2">
         <v>45552</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C12">
         <v>160.0899963378906</v>
@@ -766,19 +694,13 @@
       <c r="G12">
         <v>12064800</v>
       </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="2">
         <v>45553</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C13">
         <v>160.8500061035156</v>
@@ -795,19 +717,13 @@
       <c r="G13">
         <v>16756500</v>
       </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="2">
         <v>45554</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C14">
         <v>164.8200073242188</v>
@@ -824,19 +740,13 @@
       <c r="G14">
         <v>17548200</v>
       </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="2">
         <v>45555</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C15">
         <v>164.5200042724609</v>
@@ -853,19 +763,13 @@
       <c r="G15">
         <v>46362700</v>
       </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="2">
         <v>45558</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C16">
         <v>165.3399963378906</v>
@@ -882,19 +786,13 @@
       <c r="G16">
         <v>15648400</v>
       </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="2">
         <v>45559</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C17">
         <v>164.25</v>
@@ -911,19 +809,13 @@
       <c r="G17">
         <v>18774100</v>
       </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="2">
         <v>45560</v>
       </c>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C18">
         <v>162.9700012207031</v>
@@ -940,19 +832,13 @@
       <c r="G18">
         <v>13607900</v>
       </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="2">
         <v>45561</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C19">
         <v>165.0299987792969</v>
@@ -969,19 +855,13 @@
       <c r="G19">
         <v>18234500</v>
       </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="2">
         <v>45562</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C20">
         <v>163.9100036621094</v>
@@ -998,19 +878,13 @@
       <c r="G20">
         <v>13604300</v>
       </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="2">
         <v>45565</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C21">
         <v>164.7799987792969</v>
@@ -1027,19 +901,13 @@
       <c r="G21">
         <v>14070100</v>
       </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="2">
         <v>45566</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C22">
         <v>168.8600006103516</v>
@@ -1051,16 +919,10 @@
         <v>165.906005859375</v>
       </c>
       <c r="F22">
-        <v>168.9299926757812</v>
+        <v>168.8101043701172</v>
       </c>
       <c r="G22">
-        <v>12989676</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
+        <v>13065359</v>
       </c>
     </row>
   </sheetData>
@@ -1070,15 +932,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1098,19 +960,13 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>45538</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>228.5500030517578</v>
@@ -1127,19 +983,13 @@
       <c r="G2">
         <v>50190600</v>
       </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>45539</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>221.6600036621094</v>
@@ -1156,19 +1006,13 @@
       <c r="G3">
         <v>43840200</v>
       </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>45540</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>221.6300048828125</v>
@@ -1185,19 +1029,13 @@
       <c r="G4">
         <v>36615400</v>
       </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>45541</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>223.9499969482422</v>
@@ -1214,19 +1052,13 @@
       <c r="G5">
         <v>48423000</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>45544</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <v>220.8200073242188</v>
@@ -1243,19 +1075,13 @@
       <c r="G6">
         <v>67180000</v>
       </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>45545</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7">
         <v>218.9199981689453</v>
@@ -1272,19 +1098,13 @@
       <c r="G7">
         <v>51591000</v>
       </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>45546</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <v>221.4600067138672</v>
@@ -1301,19 +1121,13 @@
       <c r="G8">
         <v>44587100</v>
       </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>45547</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9">
         <v>222.5</v>
@@ -1330,19 +1144,13 @@
       <c r="G9">
         <v>37498200</v>
       </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="2">
         <v>45548</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10">
         <v>223.5800018310547</v>
@@ -1359,19 +1167,13 @@
       <c r="G10">
         <v>36766600</v>
       </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="2">
         <v>45551</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C11">
         <v>216.5399932861328</v>
@@ -1388,19 +1190,13 @@
       <c r="G11">
         <v>59357400</v>
       </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="2">
         <v>45552</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C12">
         <v>215.75</v>
@@ -1417,19 +1213,13 @@
       <c r="G12">
         <v>45519300</v>
       </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="2">
         <v>45553</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C13">
         <v>217.5500030517578</v>
@@ -1446,19 +1236,13 @@
       <c r="G13">
         <v>59894900</v>
       </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="2">
         <v>45554</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C14">
         <v>224.9900054931641</v>
@@ -1475,19 +1259,13 @@
       <c r="G14">
         <v>66781300</v>
       </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="2">
         <v>45555</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C15">
         <v>229.9700012207031</v>
@@ -1504,19 +1282,13 @@
       <c r="G15">
         <v>318679900</v>
       </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="2">
         <v>45558</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C16">
         <v>227.3399963378906</v>
@@ -1533,19 +1305,13 @@
       <c r="G16">
         <v>54146000</v>
       </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="2">
         <v>45559</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C17">
         <v>228.6499938964844</v>
@@ -1562,19 +1328,13 @@
       <c r="G17">
         <v>43556100</v>
       </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="2">
         <v>45560</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C18">
         <v>224.9299926757812</v>
@@ -1591,19 +1351,13 @@
       <c r="G18">
         <v>42308700</v>
       </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="2">
         <v>45561</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C19">
         <v>227.3000030517578</v>
@@ -1620,19 +1374,13 @@
       <c r="G19">
         <v>36636700</v>
       </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="2">
         <v>45562</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C20">
         <v>228.4600067138672</v>
@@ -1649,19 +1397,13 @@
       <c r="G20">
         <v>34026000</v>
       </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="2">
         <v>45565</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C21">
         <v>230.0399932861328</v>
@@ -1678,19 +1420,13 @@
       <c r="G21">
         <v>54541900</v>
       </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="2">
         <v>45566</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C22">
         <v>229.5500030517578</v>
@@ -1702,16 +1438,10 @@
         <v>223.7400054931641</v>
       </c>
       <c r="F22">
-        <v>226.1000061035156</v>
+        <v>226.0998992919922</v>
       </c>
       <c r="G22">
-        <v>43430083</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
+        <v>43997155</v>
       </c>
     </row>
   </sheetData>
@@ -1721,15 +1451,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1749,19 +1479,13 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>45538</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>177.5500030517578</v>
@@ -1778,19 +1502,13 @@
       <c r="G2">
         <v>37817500</v>
       </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>45539</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>174.4799957275391</v>
@@ -1807,19 +1525,13 @@
       <c r="G3">
         <v>30309200</v>
       </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>45540</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <v>175</v>
@@ -1836,19 +1548,13 @@
       <c r="G4">
         <v>40170500</v>
       </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>45541</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <v>177.2400054931641</v>
@@ -1865,19 +1571,13 @@
       <c r="G5">
         <v>41466500</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>45544</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <v>174.5299987792969</v>
@@ -1894,19 +1594,13 @@
       <c r="G6">
         <v>29037400</v>
       </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>45545</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>177.4900054931641</v>
@@ -1923,19 +1617,13 @@
       <c r="G7">
         <v>36233800</v>
       </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>45546</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>180.1000061035156</v>
@@ -1952,19 +1640,13 @@
       <c r="G8">
         <v>42564700</v>
       </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>45547</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <v>184.8000030517578</v>
@@ -1981,19 +1663,13 @@
       <c r="G9">
         <v>33622500</v>
       </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="2">
         <v>45548</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>187</v>
@@ -2010,19 +1686,13 @@
       <c r="G10">
         <v>26495400</v>
       </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="2">
         <v>45551</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C11">
         <v>185.2899932861328</v>
@@ -2039,19 +1709,13 @@
       <c r="G11">
         <v>26065500</v>
       </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="2">
         <v>45552</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12">
         <v>186.8500061035156</v>
@@ -2068,19 +1732,13 @@
       <c r="G12">
         <v>26091700</v>
       </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="2">
         <v>45553</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C13">
         <v>186.4499969482422</v>
@@ -2097,19 +1755,13 @@
       <c r="G13">
         <v>34448100</v>
       </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="2">
         <v>45554</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C14">
         <v>190.0399932861328</v>
@@ -2126,19 +1778,13 @@
       <c r="G14">
         <v>39543200</v>
       </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="2">
         <v>45555</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C15">
         <v>190.2299957275391</v>
@@ -2155,19 +1801,13 @@
       <c r="G15">
         <v>100378600</v>
       </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="2">
         <v>45558</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C16">
         <v>191.6399993896484</v>
@@ -2184,19 +1824,13 @@
       <c r="G16">
         <v>36993100</v>
       </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="2">
         <v>45559</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C17">
         <v>194.2700042724609</v>
@@ -2213,19 +1847,13 @@
       <c r="G17">
         <v>43478900</v>
       </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="2">
         <v>45560</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C18">
         <v>193.75</v>
@@ -2242,19 +1870,13 @@
       <c r="G18">
         <v>26391100</v>
       </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="2">
         <v>45561</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C19">
         <v>194.3099975585938</v>
@@ -2271,19 +1893,13 @@
       <c r="G19">
         <v>36334900</v>
       </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="2">
         <v>45562</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C20">
         <v>190.6799926757812</v>
@@ -2300,19 +1916,13 @@
       <c r="G20">
         <v>36002300</v>
       </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="2">
         <v>45565</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C21">
         <v>187.1399993896484</v>
@@ -2329,40 +1939,28 @@
       <c r="G21">
         <v>41583900</v>
       </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="2">
         <v>45566</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C22">
         <v>184.9600067138672</v>
       </c>
       <c r="D22">
-        <v>185.6900024414062</v>
+        <v>185.9900054931641</v>
       </c>
       <c r="E22">
         <v>183.451904296875</v>
       </c>
       <c r="F22">
-        <v>185.8099975585938</v>
+        <v>185.8699951171875</v>
       </c>
       <c r="G22">
-        <v>25100785</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
+        <v>25308146</v>
       </c>
     </row>
   </sheetData>
@@ -2372,15 +1970,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2400,19 +1998,13 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>45538</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>417.9100036621094</v>
@@ -2429,19 +2021,13 @@
       <c r="G2">
         <v>20313600</v>
       </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>45539</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>405.9100036621094</v>
@@ -2458,19 +2044,13 @@
       <c r="G3">
         <v>15135800</v>
       </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>45540</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>407.6199951171875</v>
@@ -2487,19 +2067,13 @@
       <c r="G4">
         <v>14195500</v>
       </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>45541</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>409.0599975585938</v>
@@ -2516,19 +2090,13 @@
       <c r="G5">
         <v>19609500</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>45544</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>407.239990234375</v>
@@ -2545,19 +2113,13 @@
       <c r="G6">
         <v>15295100</v>
       </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>45545</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>408.2000122070312</v>
@@ -2574,19 +2136,13 @@
       <c r="G7">
         <v>19594300</v>
       </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>45546</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C8">
         <v>415.5</v>
@@ -2603,19 +2159,13 @@
       <c r="G8">
         <v>19266900</v>
       </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>45547</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <v>423.3099975585938</v>
@@ -2632,19 +2182,13 @@
       <c r="G9">
         <v>17418800</v>
       </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="2">
         <v>45548</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <v>425.8299865722656</v>
@@ -2661,19 +2205,13 @@
       <c r="G10">
         <v>15874600</v>
       </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="2">
         <v>45551</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>430.6000061035156</v>
@@ -2690,19 +2228,13 @@
       <c r="G11">
         <v>13834700</v>
       </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="2">
         <v>45552</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C12">
         <v>440.2300109863281</v>
@@ -2719,19 +2251,13 @@
       <c r="G12">
         <v>18874200</v>
       </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="2">
         <v>45553</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C13">
         <v>435</v>
@@ -2748,19 +2274,13 @@
       <c r="G13">
         <v>18898000</v>
       </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="2">
         <v>45554</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C14">
         <v>441.2300109863281</v>
@@ -2777,19 +2297,13 @@
       <c r="G14">
         <v>21706600</v>
       </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="2">
         <v>45555</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C15">
         <v>437.2200012207031</v>
@@ -2806,19 +2320,13 @@
       <c r="G15">
         <v>55167100</v>
       </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="2">
         <v>45558</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C16">
         <v>434.2799987792969</v>
@@ -2835,19 +2343,13 @@
       <c r="G16">
         <v>15128900</v>
       </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="2">
         <v>45559</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C17">
         <v>433</v>
@@ -2864,19 +2366,13 @@
       <c r="G17">
         <v>17015800</v>
       </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="2">
         <v>45560</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C18">
         <v>429.8299865722656</v>
@@ -2893,19 +2389,13 @@
       <c r="G18">
         <v>13396400</v>
       </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="2">
         <v>45561</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C19">
         <v>435.0899963378906</v>
@@ -2922,19 +2412,13 @@
       <c r="G19">
         <v>14492000</v>
       </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="2">
         <v>45562</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C20">
         <v>431.5199890136719</v>
@@ -2951,19 +2435,13 @@
       <c r="G20">
         <v>14896100</v>
       </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="2">
         <v>45565</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C21">
         <v>428.2099914550781</v>
@@ -2980,19 +2458,13 @@
       <c r="G21">
         <v>16807300</v>
       </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="2">
         <v>45566</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C22">
         <v>428.3800048828125</v>
@@ -3001,19 +2473,13 @@
         <v>428.4700012207031</v>
       </c>
       <c r="E22">
-        <v>419.5299987792969</v>
+        <v>418.8250122070312</v>
       </c>
       <c r="F22">
-        <v>422.49169921875</v>
+        <v>422.5599975585938</v>
       </c>
       <c r="G22">
-        <v>11603405</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
+        <v>11694962</v>
       </c>
     </row>
   </sheetData>

</xml_diff>